<commit_message>
main list dir in root
</commit_message>
<xml_diff>
--- a/Summary/SIT-00016/Summary_SIT-00016.xlsx
+++ b/Summary/SIT-00016/Summary_SIT-00016.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:BF2"/>
+  <dimension ref="A1:BF5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1017,6 +1017,882 @@
         </is>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>SIT-00016</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>2024-03-18</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>09:36:59</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>REVISE</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>['HOME ?-29 : (114.009346, -7.691572000000011)']</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>['HOME ?-1 : (114.010231, -7.692147000000005)', 'HOME ?-29 : (114.009346, -7.691572000000011)', 'HOME ?-49 : (114.006126, -7.691618)', 'HOME 5 : (114.006401, -7.692279000000015)', 'HOME 14 : (114.006065, -7.692483000000008)', 'HOME 13 : (114.006142, -7.69239099999999)', 'HOME ?-56 : (114.006233, -7.692200000000014)', 'HOME 9* : (114.006256, -7.692561000000007)', 'HOME 12 : (114.006157, -7.692311999999988)', 'HOME 11 : (114.006233, -7.692688000000003)', 'HOME ?-117 : (114.00631, -7.692485000000014)', 'HOME ?-146 : (114.008286, -7.69253)', 'HOME ?-150 : (114.010101, -7.692127999999991)', 'HOME ?-153 : (114.010132, -7.692245000000019)', 'HOME ?-163 : (114.009918, -7.692179000000015)', 'HOME ?-169 : (114.010099, -7.692218999999987)', 'HOME ?-170 : (114.009888, -7.692055000000007)', 'HOME ?-179 : (114.010033, -7.692185999999994)', 'HOME ?-180 : (114.008224, -7.692498000000009)', 'HOME ?-183 : (114.009857, -7.692186999999997)', 'HOME ?-186 : (114.009979, -7.692085999999994)', 'HOME ?-187 : (114.010155, -7.692352)', 'HOME 149 : (114.010132, -7.692450999999998)', 'HOME ?-207 : (114.009979, -7.692191000000008)']</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="L3" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="M3" t="inlineStr">
+        <is>
+          <t>Revise</t>
+        </is>
+      </c>
+      <c r="N3" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="O3" t="inlineStr">
+        <is>
+          <t>Revise</t>
+        </is>
+      </c>
+      <c r="P3" t="inlineStr">
+        <is>
+          <t>Revise</t>
+        </is>
+      </c>
+      <c r="Q3" t="inlineStr">
+        <is>
+          <t>Revise</t>
+        </is>
+      </c>
+      <c r="R3" t="inlineStr">
+        <is>
+          <t>Revise</t>
+        </is>
+      </c>
+      <c r="S3" t="inlineStr">
+        <is>
+          <t>Revise</t>
+        </is>
+      </c>
+      <c r="T3" t="inlineStr">
+        <is>
+          <t>Revise</t>
+        </is>
+      </c>
+      <c r="U3" t="inlineStr">
+        <is>
+          <t>Revise</t>
+        </is>
+      </c>
+      <c r="V3" t="inlineStr">
+        <is>
+          <t>Revise</t>
+        </is>
+      </c>
+      <c r="W3" t="inlineStr">
+        <is>
+          <t>Revise</t>
+        </is>
+      </c>
+      <c r="X3" t="inlineStr">
+        <is>
+          <t>Revise</t>
+        </is>
+      </c>
+      <c r="Y3" t="inlineStr">
+        <is>
+          <t>Revise</t>
+        </is>
+      </c>
+      <c r="Z3" t="inlineStr">
+        <is>
+          <t>Revise</t>
+        </is>
+      </c>
+      <c r="AA3" t="inlineStr">
+        <is>
+          <t>Revise</t>
+        </is>
+      </c>
+      <c r="AB3" t="inlineStr">
+        <is>
+          <t>Revise</t>
+        </is>
+      </c>
+      <c r="AC3" t="inlineStr">
+        <is>
+          <t>Revise</t>
+        </is>
+      </c>
+      <c r="AD3" t="inlineStr">
+        <is>
+          <t>Revise</t>
+        </is>
+      </c>
+      <c r="AE3" t="inlineStr">
+        <is>
+          <t>Revise</t>
+        </is>
+      </c>
+      <c r="AF3" t="inlineStr">
+        <is>
+          <t>Revise</t>
+        </is>
+      </c>
+      <c r="AG3" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="AH3" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="AI3" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="AJ3" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="AK3" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="AL3" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="AM3" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="AN3" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="AO3" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="AP3" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="AQ3" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="AR3" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="AS3" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="AT3" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="AU3" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="AV3" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="AW3" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="AX3" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="AY3" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="AZ3" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="BA3" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="BB3" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="BC3" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="BD3" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="BE3" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="BF3" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>SIT-00016</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>2024-03-18</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>09:39:55</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>REVISE</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>['HOME ?-29 : (114.009346, -7.691572000000011)']</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>['HOME ?-1 : (114.010231, -7.692147000000005)', 'HOME ?-29 : (114.009346, -7.691572000000011)', 'HOME ?-49 : (114.006126, -7.691618)', 'HOME 5 : (114.006401, -7.692279000000015)', 'HOME 14 : (114.006065, -7.692483000000008)', 'HOME 13 : (114.006142, -7.69239099999999)', 'HOME ?-56 : (114.006233, -7.692200000000014)', 'HOME 9* : (114.006256, -7.692561000000007)', 'HOME 12 : (114.006157, -7.692311999999988)', 'HOME 11 : (114.006233, -7.692688000000003)', 'HOME ?-117 : (114.00631, -7.692485000000014)', 'HOME ?-146 : (114.008286, -7.69253)', 'HOME ?-150 : (114.010101, -7.692127999999991)', 'HOME ?-153 : (114.010132, -7.692245000000019)', 'HOME ?-163 : (114.009918, -7.692179000000015)', 'HOME ?-169 : (114.010099, -7.692218999999987)', 'HOME ?-170 : (114.009888, -7.692055000000007)', 'HOME ?-179 : (114.010033, -7.692185999999994)', 'HOME ?-180 : (114.008224, -7.692498000000009)', 'HOME ?-183 : (114.009857, -7.692186999999997)', 'HOME ?-186 : (114.009979, -7.692085999999994)', 'HOME ?-187 : (114.010155, -7.692352)', 'HOME 149 : (114.010132, -7.692450999999998)', 'HOME ?-207 : (114.009979, -7.692191000000008)']</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="L4" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="M4" t="inlineStr">
+        <is>
+          <t>Revise</t>
+        </is>
+      </c>
+      <c r="N4" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="O4" t="inlineStr">
+        <is>
+          <t>Revise</t>
+        </is>
+      </c>
+      <c r="P4" t="inlineStr">
+        <is>
+          <t>Revise</t>
+        </is>
+      </c>
+      <c r="Q4" t="inlineStr">
+        <is>
+          <t>Revise</t>
+        </is>
+      </c>
+      <c r="R4" t="inlineStr">
+        <is>
+          <t>Revise</t>
+        </is>
+      </c>
+      <c r="S4" t="inlineStr">
+        <is>
+          <t>Revise</t>
+        </is>
+      </c>
+      <c r="T4" t="inlineStr">
+        <is>
+          <t>Revise</t>
+        </is>
+      </c>
+      <c r="U4" t="inlineStr">
+        <is>
+          <t>Revise</t>
+        </is>
+      </c>
+      <c r="V4" t="inlineStr">
+        <is>
+          <t>Revise</t>
+        </is>
+      </c>
+      <c r="W4" t="inlineStr">
+        <is>
+          <t>Revise</t>
+        </is>
+      </c>
+      <c r="X4" t="inlineStr">
+        <is>
+          <t>Revise</t>
+        </is>
+      </c>
+      <c r="Y4" t="inlineStr">
+        <is>
+          <t>Revise</t>
+        </is>
+      </c>
+      <c r="Z4" t="inlineStr">
+        <is>
+          <t>Revise</t>
+        </is>
+      </c>
+      <c r="AA4" t="inlineStr">
+        <is>
+          <t>Revise</t>
+        </is>
+      </c>
+      <c r="AB4" t="inlineStr">
+        <is>
+          <t>Revise</t>
+        </is>
+      </c>
+      <c r="AC4" t="inlineStr">
+        <is>
+          <t>Revise</t>
+        </is>
+      </c>
+      <c r="AD4" t="inlineStr">
+        <is>
+          <t>Revise</t>
+        </is>
+      </c>
+      <c r="AE4" t="inlineStr">
+        <is>
+          <t>Revise</t>
+        </is>
+      </c>
+      <c r="AF4" t="inlineStr">
+        <is>
+          <t>Revise</t>
+        </is>
+      </c>
+      <c r="AG4" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="AH4" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="AI4" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="AJ4" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="AK4" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="AL4" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="AM4" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="AN4" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="AO4" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="AP4" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="AQ4" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="AR4" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="AS4" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="AT4" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="AU4" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="AV4" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="AW4" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="AX4" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="AY4" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="AZ4" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="BA4" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="BB4" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="BC4" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="BD4" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="BE4" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="BF4" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>SIT-00016</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>2024-03-18</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>09:49:55</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>REVISE</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>['HOME ?-29 : (114.009346, -7.691572000000011)']</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>['HOME ?-1 : (114.010231, -7.692147000000005)', 'HOME ?-29 : (114.009346, -7.691572000000011)', 'HOME ?-49 : (114.006126, -7.691618)', 'HOME 5 : (114.006401, -7.692279000000015)', 'HOME 14 : (114.006065, -7.692483000000008)', 'HOME 13 : (114.006142, -7.69239099999999)', 'HOME ?-56 : (114.006233, -7.692200000000014)', 'HOME 9* : (114.006256, -7.692561000000007)', 'HOME 12 : (114.006157, -7.692311999999988)', 'HOME 11 : (114.006233, -7.692688000000003)', 'HOME ?-117 : (114.00631, -7.692485000000014)', 'HOME ?-146 : (114.008286, -7.69253)', 'HOME ?-150 : (114.010101, -7.692127999999991)', 'HOME ?-153 : (114.010132, -7.692245000000019)', 'HOME ?-163 : (114.009918, -7.692179000000015)', 'HOME ?-169 : (114.010099, -7.692218999999987)', 'HOME ?-170 : (114.009888, -7.692055000000007)', 'HOME ?-179 : (114.010033, -7.692185999999994)', 'HOME ?-180 : (114.008224, -7.692498000000009)', 'HOME ?-183 : (114.009857, -7.692186999999997)', 'HOME ?-186 : (114.009979, -7.692085999999994)', 'HOME ?-187 : (114.010155, -7.692352)', 'HOME 149 : (114.010132, -7.692450999999998)', 'HOME ?-207 : (114.009979, -7.692191000000008)']</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="L5" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="M5" t="inlineStr">
+        <is>
+          <t>Revise</t>
+        </is>
+      </c>
+      <c r="N5" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="O5" t="inlineStr">
+        <is>
+          <t>Revise</t>
+        </is>
+      </c>
+      <c r="P5" t="inlineStr">
+        <is>
+          <t>Revise</t>
+        </is>
+      </c>
+      <c r="Q5" t="inlineStr">
+        <is>
+          <t>Revise</t>
+        </is>
+      </c>
+      <c r="R5" t="inlineStr">
+        <is>
+          <t>Revise</t>
+        </is>
+      </c>
+      <c r="S5" t="inlineStr">
+        <is>
+          <t>Revise</t>
+        </is>
+      </c>
+      <c r="T5" t="inlineStr">
+        <is>
+          <t>Revise</t>
+        </is>
+      </c>
+      <c r="U5" t="inlineStr">
+        <is>
+          <t>Revise</t>
+        </is>
+      </c>
+      <c r="V5" t="inlineStr">
+        <is>
+          <t>Revise</t>
+        </is>
+      </c>
+      <c r="W5" t="inlineStr">
+        <is>
+          <t>Revise</t>
+        </is>
+      </c>
+      <c r="X5" t="inlineStr">
+        <is>
+          <t>Revise</t>
+        </is>
+      </c>
+      <c r="Y5" t="inlineStr">
+        <is>
+          <t>Revise</t>
+        </is>
+      </c>
+      <c r="Z5" t="inlineStr">
+        <is>
+          <t>Revise</t>
+        </is>
+      </c>
+      <c r="AA5" t="inlineStr">
+        <is>
+          <t>Revise</t>
+        </is>
+      </c>
+      <c r="AB5" t="inlineStr">
+        <is>
+          <t>Revise</t>
+        </is>
+      </c>
+      <c r="AC5" t="inlineStr">
+        <is>
+          <t>Revise</t>
+        </is>
+      </c>
+      <c r="AD5" t="inlineStr">
+        <is>
+          <t>Revise</t>
+        </is>
+      </c>
+      <c r="AE5" t="inlineStr">
+        <is>
+          <t>Revise</t>
+        </is>
+      </c>
+      <c r="AF5" t="inlineStr">
+        <is>
+          <t>Revise</t>
+        </is>
+      </c>
+      <c r="AG5" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="AH5" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="AI5" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="AJ5" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="AK5" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="AL5" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="AM5" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="AN5" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="AO5" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="AP5" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="AQ5" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="AR5" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="AS5" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="AT5" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="AU5" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="AV5" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="AW5" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="AX5" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="AY5" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="AZ5" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="BA5" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="BB5" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="BC5" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="BD5" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="BE5" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="BF5" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
update list dir logic
</commit_message>
<xml_diff>
--- a/Summary/SIT-00016/Summary_SIT-00016.xlsx
+++ b/Summary/SIT-00016/Summary_SIT-00016.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:BF5"/>
+  <dimension ref="A1:BF6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1893,6 +1893,298 @@
         </is>
       </c>
     </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>SIT-00016</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>2024-03-18</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>10:33:28</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>REVISE</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>['HOME ?-29 : (114.009346, -7.691572000000011)']</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>['HOME ?-1 : (114.010231, -7.692147000000005)', 'HOME ?-29 : (114.009346, -7.691572000000011)', 'HOME ?-49 : (114.006126, -7.691618)', 'HOME 5 : (114.006401, -7.692279000000015)', 'HOME 14 : (114.006065, -7.692483000000008)', 'HOME 13 : (114.006142, -7.69239099999999)', 'HOME ?-56 : (114.006233, -7.692200000000014)', 'HOME 9* : (114.006256, -7.692561000000007)', 'HOME 12 : (114.006157, -7.692311999999988)', 'HOME 11 : (114.006233, -7.692688000000003)', 'HOME ?-117 : (114.00631, -7.692485000000014)', 'HOME ?-146 : (114.008286, -7.69253)', 'HOME ?-150 : (114.010101, -7.692127999999991)', 'HOME ?-153 : (114.010132, -7.692245000000019)', 'HOME ?-163 : (114.009918, -7.692179000000015)', 'HOME ?-169 : (114.010099, -7.692218999999987)', 'HOME ?-170 : (114.009888, -7.692055000000007)', 'HOME ?-179 : (114.010033, -7.692185999999994)', 'HOME ?-180 : (114.008224, -7.692498000000009)', 'HOME ?-183 : (114.009857, -7.692186999999997)', 'HOME ?-186 : (114.009979, -7.692085999999994)', 'HOME ?-187 : (114.010155, -7.692352)', 'HOME 149 : (114.010132, -7.692450999999998)', 'HOME ?-207 : (114.009979, -7.692191000000008)']</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="K6" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="L6" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="M6" t="inlineStr">
+        <is>
+          <t>Revise</t>
+        </is>
+      </c>
+      <c r="N6" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="O6" t="inlineStr">
+        <is>
+          <t>Revise</t>
+        </is>
+      </c>
+      <c r="P6" t="inlineStr">
+        <is>
+          <t>Revise</t>
+        </is>
+      </c>
+      <c r="Q6" t="inlineStr">
+        <is>
+          <t>Revise</t>
+        </is>
+      </c>
+      <c r="R6" t="inlineStr">
+        <is>
+          <t>Revise</t>
+        </is>
+      </c>
+      <c r="S6" t="inlineStr">
+        <is>
+          <t>Revise</t>
+        </is>
+      </c>
+      <c r="T6" t="inlineStr">
+        <is>
+          <t>Revise</t>
+        </is>
+      </c>
+      <c r="U6" t="inlineStr">
+        <is>
+          <t>Revise</t>
+        </is>
+      </c>
+      <c r="V6" t="inlineStr">
+        <is>
+          <t>Revise</t>
+        </is>
+      </c>
+      <c r="W6" t="inlineStr">
+        <is>
+          <t>Revise</t>
+        </is>
+      </c>
+      <c r="X6" t="inlineStr">
+        <is>
+          <t>Revise</t>
+        </is>
+      </c>
+      <c r="Y6" t="inlineStr">
+        <is>
+          <t>Revise</t>
+        </is>
+      </c>
+      <c r="Z6" t="inlineStr">
+        <is>
+          <t>Revise</t>
+        </is>
+      </c>
+      <c r="AA6" t="inlineStr">
+        <is>
+          <t>Revise</t>
+        </is>
+      </c>
+      <c r="AB6" t="inlineStr">
+        <is>
+          <t>Revise</t>
+        </is>
+      </c>
+      <c r="AC6" t="inlineStr">
+        <is>
+          <t>Revise</t>
+        </is>
+      </c>
+      <c r="AD6" t="inlineStr">
+        <is>
+          <t>Revise</t>
+        </is>
+      </c>
+      <c r="AE6" t="inlineStr">
+        <is>
+          <t>Revise</t>
+        </is>
+      </c>
+      <c r="AF6" t="inlineStr">
+        <is>
+          <t>Revise</t>
+        </is>
+      </c>
+      <c r="AG6" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="AH6" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="AI6" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="AJ6" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="AK6" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="AL6" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="AM6" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="AN6" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="AO6" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="AP6" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="AQ6" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="AR6" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="AS6" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="AT6" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="AU6" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="AV6" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="AW6" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="AX6" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="AY6" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="AZ6" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="BA6" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="BB6" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="BC6" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="BD6" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="BE6" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="BF6" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>